<commit_message>
adding latest metadata from Anna
</commit_message>
<xml_diff>
--- a/src/data/FoodbornePathogenDetectionDataAnalysis.xlsx
+++ b/src/data/FoodbornePathogenDetectionDataAnalysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="464">
   <si>
     <t>Galaxy ID</t>
   </si>
@@ -1685,6 +1685,18 @@
   </si>
   <si>
     <t>2.4E+6 CFU/ml S. salameae</t>
+  </si>
+  <si>
+    <t>Mixes were made with</t>
+  </si>
+  <si>
+    <t>S. hout</t>
+  </si>
+  <si>
+    <t>S. salam</t>
+  </si>
+  <si>
+    <t>S. ent</t>
   </si>
 </sst>
 </file>
@@ -1885,6 +1897,9 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -1893,9 +1908,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -2345,7 +2357,9 @@
       <c r="L3" s="6">
         <v>24.0</v>
       </c>
-      <c r="M3" s="6"/>
+      <c r="M3" s="12">
+        <v>5.8E7</v>
+      </c>
       <c r="N3" s="6" t="s">
         <v>28</v>
       </c>
@@ -2388,7 +2402,9 @@
       <c r="L4" s="6">
         <v>19.0</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="12">
+        <v>5.8E8</v>
+      </c>
       <c r="N4" s="6" t="s">
         <v>28</v>
       </c>
@@ -2472,7 +2488,9 @@
       <c r="L6" s="6">
         <v>27.0</v>
       </c>
-      <c r="M6" s="3"/>
+      <c r="M6" s="12">
+        <v>5800000.0</v>
+      </c>
       <c r="N6" s="6" t="s">
         <v>50</v>
       </c>
@@ -2515,7 +2533,9 @@
       <c r="L7" s="6">
         <v>29.0</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="12">
+        <v>580000.0</v>
+      </c>
       <c r="N7" s="6" t="s">
         <v>50</v>
       </c>
@@ -2524,25 +2544,25 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -2558,7 +2578,7 @@
       <c r="L8" s="6">
         <v>13.0</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="12">
         <v>1.05E12</v>
       </c>
       <c r="N8" s="6" t="s">
@@ -2571,25 +2591,25 @@
       <c r="Q8" s="10"/>
     </row>
     <row r="9">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>63</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -2605,7 +2625,7 @@
       <c r="L9" s="6">
         <v>21.0</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="12">
         <v>1.11E9</v>
       </c>
       <c r="N9" s="6" t="s">
@@ -2616,25 +2636,25 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>66</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -2650,7 +2670,7 @@
       <c r="L10" s="6">
         <v>18.0</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="12">
         <v>9.0E7</v>
       </c>
       <c r="N10" s="6" t="s">
@@ -2661,25 +2681,25 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="13" t="s">
         <v>69</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -2695,7 +2715,7 @@
       <c r="L11" s="6">
         <v>28.0</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="12">
         <v>1200000.0</v>
       </c>
       <c r="N11" s="6" t="s">
@@ -2706,25 +2726,25 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -2740,7 +2760,7 @@
       <c r="L12" s="6">
         <v>28.0</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="12">
         <v>68000.0</v>
       </c>
       <c r="N12" s="6" t="s">
@@ -2751,25 +2771,25 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -2785,7 +2805,7 @@
       <c r="L13" s="6">
         <v>30.0</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="12">
         <v>24000.0</v>
       </c>
       <c r="N13" s="6" t="s">
@@ -2796,25 +2816,25 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>75</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -2830,7 +2850,7 @@
       <c r="L14" s="6">
         <v>13.0</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="12">
         <v>1.05E12</v>
       </c>
       <c r="N14" s="6" t="s">
@@ -2843,25 +2863,25 @@
       <c r="Q14" s="10"/>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>79</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -2877,7 +2897,7 @@
       <c r="L15" s="6">
         <v>21.0</v>
       </c>
-      <c r="M15" s="15">
+      <c r="M15" s="12">
         <v>1.11E9</v>
       </c>
       <c r="N15" s="6" t="s">
@@ -2888,25 +2908,25 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="13" t="s">
         <v>82</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -2922,7 +2942,7 @@
       <c r="L16" s="6">
         <v>18.0</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16" s="12">
         <v>9.0E7</v>
       </c>
       <c r="N16" s="6" t="s">
@@ -2933,25 +2953,25 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>85</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -2967,7 +2987,7 @@
       <c r="L17" s="6">
         <v>28.0</v>
       </c>
-      <c r="M17" s="15">
+      <c r="M17" s="12">
         <v>1200000.0</v>
       </c>
       <c r="N17" s="6" t="s">
@@ -2978,25 +2998,25 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="13" t="s">
         <v>87</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -3012,7 +3032,7 @@
       <c r="L18" s="6">
         <v>28.0</v>
       </c>
-      <c r="M18" s="15">
+      <c r="M18" s="12">
         <v>68000.0</v>
       </c>
       <c r="N18" s="6" t="s">
@@ -3023,25 +3043,25 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="13" t="s">
         <v>89</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -3057,7 +3077,7 @@
       <c r="L19" s="6">
         <v>30.0</v>
       </c>
-      <c r="M19" s="15">
+      <c r="M19" s="12">
         <v>24000.0</v>
       </c>
       <c r="N19" s="6" t="s">
@@ -3068,7 +3088,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>91</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -3080,7 +3100,7 @@
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -3097,25 +3117,25 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="13" t="s">
         <v>94</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -3133,7 +3153,7 @@
       <c r="L21" s="6">
         <v>13.0</v>
       </c>
-      <c r="M21" s="15">
+      <c r="M21" s="12">
         <v>1.05E12</v>
       </c>
       <c r="N21" s="6" t="s">
@@ -3149,28 +3169,28 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>99</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I22" s="6" t="s">
@@ -3185,7 +3205,7 @@
       <c r="L22" s="6">
         <v>21.0</v>
       </c>
-      <c r="M22" s="15">
+      <c r="M22" s="12">
         <v>1.11E9</v>
       </c>
       <c r="N22" s="6" t="s">
@@ -3196,28 +3216,28 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="13" t="s">
         <v>102</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I23" s="6" t="s">
@@ -3232,7 +3252,7 @@
       <c r="L23" s="6">
         <v>18.0</v>
       </c>
-      <c r="M23" s="15">
+      <c r="M23" s="12">
         <v>9.0E7</v>
       </c>
       <c r="N23" s="6" t="s">
@@ -3243,28 +3263,28 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="13" t="s">
         <v>105</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G24" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="H24" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I24" s="6" t="s">
@@ -3279,7 +3299,7 @@
       <c r="L24" s="6">
         <v>28.0</v>
       </c>
-      <c r="M24" s="15">
+      <c r="M24" s="12">
         <v>1200000.0</v>
       </c>
       <c r="N24" s="6" t="s">
@@ -3290,28 +3310,28 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>108</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="H25" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I25" s="11" t="s">
@@ -3326,7 +3346,7 @@
       <c r="L25" s="6">
         <v>28.0</v>
       </c>
-      <c r="M25" s="15">
+      <c r="M25" s="12">
         <v>68000.0</v>
       </c>
       <c r="N25" s="6" t="s">
@@ -3337,28 +3357,28 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>111</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G26" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="12" t="s">
+      <c r="H26" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I26" s="11" t="s">
@@ -3373,7 +3393,7 @@
       <c r="L26" s="6">
         <v>30.0</v>
       </c>
-      <c r="M26" s="15">
+      <c r="M26" s="12">
         <v>24000.0</v>
       </c>
       <c r="N26" s="6" t="s">
@@ -3384,58 +3404,58 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="13" t="s">
         <v>114</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="13" t="s">
         <v>93</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="12" t="s">
+      <c r="I27" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12" t="s">
+      <c r="J27" s="13"/>
+      <c r="K27" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
       <c r="O27" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>117</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H28" s="2" t="s">
@@ -3454,7 +3474,7 @@
       <c r="L28" s="6">
         <v>13.0</v>
       </c>
-      <c r="M28" s="15">
+      <c r="M28" s="12">
         <v>1.05E12</v>
       </c>
       <c r="N28" s="6" t="s">
@@ -3470,28 +3490,28 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="13" t="s">
         <v>121</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I29" s="6" t="s">
@@ -3507,7 +3527,7 @@
       <c r="L29" s="6">
         <v>21.0</v>
       </c>
-      <c r="M29" s="15">
+      <c r="M29" s="12">
         <v>1.11E9</v>
       </c>
       <c r="N29" s="6" t="s">
@@ -3518,28 +3538,28 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="13" t="s">
         <v>124</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="G30" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H30" s="12" t="s">
+      <c r="H30" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I30" s="6" t="s">
@@ -3555,7 +3575,7 @@
       <c r="L30" s="6">
         <v>18.0</v>
       </c>
-      <c r="M30" s="15">
+      <c r="M30" s="12">
         <v>9.0E7</v>
       </c>
       <c r="N30" s="6" t="s">
@@ -3566,28 +3586,28 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="13" t="s">
         <v>127</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H31" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I31" s="6" t="s">
@@ -3603,7 +3623,7 @@
       <c r="L31" s="6">
         <v>28.0</v>
       </c>
-      <c r="M31" s="15">
+      <c r="M31" s="12">
         <v>1200000.0</v>
       </c>
       <c r="N31" s="6" t="s">
@@ -3614,28 +3634,28 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="13" t="s">
         <v>130</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="12" t="s">
+      <c r="H32" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I32" s="11" t="s">
@@ -3651,7 +3671,7 @@
       <c r="L32" s="6">
         <v>28.0</v>
       </c>
-      <c r="M32" s="15">
+      <c r="M32" s="12">
         <v>68000.0</v>
       </c>
       <c r="N32" s="6" t="s">
@@ -3662,28 +3682,28 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="13" t="s">
         <v>133</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G33" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="H33" s="13" t="s">
         <v>96</v>
       </c>
       <c r="I33" s="11" t="s">
@@ -3699,7 +3719,7 @@
       <c r="L33" s="6">
         <v>30.0</v>
       </c>
-      <c r="M33" s="15">
+      <c r="M33" s="12">
         <v>24000.0</v>
       </c>
       <c r="N33" s="6" t="s">
@@ -3710,34 +3730,34 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="13" t="s">
         <v>136</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="13" t="s">
         <v>93</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
-      <c r="G34" s="12" t="s">
+      <c r="G34" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="12" t="s">
+      <c r="H34" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="I34" s="12" t="s">
+      <c r="I34" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12" t="s">
+      <c r="J34" s="13"/>
+      <c r="K34" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
       <c r="O34" s="18" t="s">
         <v>29</v>
       </c>
@@ -3752,40 +3772,42 @@
       <c r="C35" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G35" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="12" t="s">
+      <c r="H35" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I35" s="13" t="s">
+      <c r="I35" s="14" t="s">
         <v>143</v>
       </c>
       <c r="J35" s="7" t="str">
         <f t="shared" ref="J35:J42" si="2">LEFT(I35,FIND(CHAR(160),SUBSTITUTE(I35," ",CHAR(160),4)) - 1)</f>
         <v>Salmonella enterica subsp. Enterica</v>
       </c>
-      <c r="K35" s="12"/>
+      <c r="K35" s="13"/>
       <c r="L35" s="6">
         <v>15.956588499999999</v>
       </c>
-      <c r="M35" s="11"/>
+      <c r="M35" s="12">
+        <v>1200000.0</v>
+      </c>
       <c r="N35" s="11" t="s">
         <v>50</v>
       </c>
       <c r="O35" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="P35" s="12"/>
+      <c r="P35" s="13"/>
       <c r="Q35" s="10"/>
       <c r="R35" s="17" t="s">
         <v>144</v>
@@ -3801,27 +3823,29 @@
       <c r="C36" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="12" t="s">
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="12" t="s">
+      <c r="H36" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="I36" s="14" t="s">
         <v>148</v>
       </c>
       <c r="J36" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Salmonella enterica subsp. Enterica</v>
       </c>
-      <c r="K36" s="12"/>
+      <c r="K36" s="13"/>
       <c r="L36" s="6">
         <v>18.498361</v>
       </c>
-      <c r="M36" s="11"/>
+      <c r="M36" s="12">
+        <v>290000.0</v>
+      </c>
       <c r="N36" s="11" t="s">
         <v>50</v>
       </c>
@@ -3839,27 +3863,29 @@
       <c r="C37" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="12" t="s">
+      <c r="D37" s="14"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="12" t="s">
+      <c r="H37" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I37" s="13" t="s">
+      <c r="I37" s="14" t="s">
         <v>152</v>
       </c>
       <c r="J37" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Salmonella enterica subsp. Enterica</v>
       </c>
-      <c r="K37" s="12"/>
+      <c r="K37" s="13"/>
       <c r="L37" s="6">
         <v>21.711907</v>
       </c>
-      <c r="M37" s="11"/>
+      <c r="M37" s="12">
+        <v>53000.0</v>
+      </c>
       <c r="N37" s="11" t="s">
         <v>50</v>
       </c>
@@ -3877,27 +3903,29 @@
       <c r="C38" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="12" t="s">
+      <c r="D38" s="14"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="12" t="s">
+      <c r="H38" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I38" s="13" t="s">
+      <c r="I38" s="14" t="s">
         <v>156</v>
       </c>
       <c r="J38" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Salmonella enterica subsp. Enterica</v>
       </c>
-      <c r="K38" s="12"/>
+      <c r="K38" s="13"/>
       <c r="L38" s="6">
         <v>25.20456</v>
       </c>
-      <c r="M38" s="11"/>
+      <c r="M38" s="12">
+        <v>1400.0</v>
+      </c>
       <c r="N38" s="11" t="s">
         <v>50</v>
       </c>
@@ -3915,33 +3943,35 @@
       <c r="C39" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G39" s="12" t="s">
+      <c r="G39" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H39" s="12" t="s">
+      <c r="H39" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I39" s="13" t="s">
+      <c r="I39" s="14" t="s">
         <v>160</v>
       </c>
       <c r="J39" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Salmonella enterica subsp. Houtenae</v>
       </c>
-      <c r="K39" s="12"/>
+      <c r="K39" s="13"/>
       <c r="L39" s="6">
         <v>24.801299969938302</v>
       </c>
-      <c r="M39" s="13"/>
+      <c r="M39" s="12">
+        <v>610000.0</v>
+      </c>
       <c r="N39" s="11" t="s">
         <v>50</v>
       </c>
@@ -3959,27 +3989,29 @@
       <c r="C40" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="12" t="s">
+      <c r="D40" s="14"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H40" s="12" t="s">
+      <c r="H40" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I40" s="13" t="s">
+      <c r="I40" s="14" t="s">
         <v>164</v>
       </c>
       <c r="J40" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Salmonella enterica subsp. Houtenae</v>
       </c>
-      <c r="K40" s="12"/>
+      <c r="K40" s="13"/>
       <c r="L40" s="6">
         <v>28.38766159953725</v>
       </c>
-      <c r="M40" s="13"/>
+      <c r="M40" s="12">
+        <v>68000.0</v>
+      </c>
       <c r="N40" s="11" t="s">
         <v>50</v>
       </c>
@@ -3997,27 +4029,29 @@
       <c r="C41" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="12" t="s">
+      <c r="D41" s="14"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H41" s="12" t="s">
+      <c r="H41" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="I41" s="14" t="s">
         <v>168</v>
       </c>
       <c r="J41" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Salmonella enterica subsp. Houtenae</v>
       </c>
-      <c r="K41" s="12"/>
+      <c r="K41" s="13"/>
       <c r="L41" s="6">
         <v>32.13181070188789</v>
       </c>
-      <c r="M41" s="13"/>
+      <c r="M41" s="12">
+        <v>6800.0</v>
+      </c>
       <c r="N41" s="11" t="s">
         <v>50</v>
       </c>
@@ -4035,27 +4069,29 @@
       <c r="C42" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="12" t="s">
+      <c r="D42" s="14"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H42" s="12" t="s">
+      <c r="H42" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I42" s="13" t="s">
+      <c r="I42" s="14" t="s">
         <v>172</v>
       </c>
       <c r="J42" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Salmonella enterica subsp. Houtenae</v>
       </c>
-      <c r="K42" s="12"/>
+      <c r="K42" s="13"/>
       <c r="L42" s="6">
         <v>46.6568</v>
       </c>
-      <c r="M42" s="13"/>
+      <c r="M42" s="12">
+        <v>810.0</v>
+      </c>
       <c r="N42" s="11" t="s">
         <v>50</v>
       </c>
@@ -4073,32 +4109,34 @@
       <c r="C43" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="F43" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G43" s="12" t="s">
+      <c r="G43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H43" s="12" t="s">
+      <c r="H43" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I43" s="13" t="s">
+      <c r="I43" s="14" t="s">
         <v>176</v>
       </c>
       <c r="J43" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="K43" s="12"/>
+      <c r="K43" s="13"/>
       <c r="L43" s="6">
         <v>30.973821499999996</v>
       </c>
-      <c r="M43" s="13"/>
+      <c r="M43" s="12">
+        <v>24000.0</v>
+      </c>
       <c r="N43" s="11" t="s">
         <v>50</v>
       </c>
@@ -4116,26 +4154,28 @@
       <c r="C44" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="D44" s="13"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="12" t="s">
+      <c r="D44" s="14"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H44" s="12" t="s">
+      <c r="H44" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I44" s="13" t="s">
+      <c r="I44" s="14" t="s">
         <v>180</v>
       </c>
       <c r="J44" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="K44" s="12"/>
+      <c r="K44" s="13"/>
       <c r="L44" s="6">
         <v>34.2050315</v>
       </c>
-      <c r="M44" s="13"/>
+      <c r="M44" s="12">
+        <v>2100.0</v>
+      </c>
       <c r="N44" s="11" t="s">
         <v>50</v>
       </c>
@@ -4153,26 +4193,28 @@
       <c r="C45" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="12" t="s">
+      <c r="D45" s="14"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H45" s="12" t="s">
+      <c r="H45" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I45" s="13" t="s">
+      <c r="I45" s="14" t="s">
         <v>184</v>
       </c>
       <c r="J45" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="K45" s="12"/>
+      <c r="K45" s="13"/>
       <c r="L45" s="6">
         <v>41.046124999999996</v>
       </c>
-      <c r="M45" s="13"/>
+      <c r="M45" s="12">
+        <v>220.0</v>
+      </c>
       <c r="N45" s="11" t="s">
         <v>50</v>
       </c>
@@ -4190,26 +4232,28 @@
       <c r="C46" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="D46" s="13"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="12" t="s">
+      <c r="D46" s="14"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H46" s="12" t="s">
+      <c r="H46" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I46" s="13" t="s">
+      <c r="I46" s="14" t="s">
         <v>188</v>
       </c>
       <c r="J46" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="K46" s="12"/>
+      <c r="K46" s="13"/>
       <c r="L46" s="6">
         <v>36.2067585</v>
       </c>
-      <c r="M46" s="13"/>
+      <c r="M46" s="12">
+        <v>10.0</v>
+      </c>
       <c r="N46" s="11" t="s">
         <v>50</v>
       </c>
@@ -4227,24 +4271,24 @@
       <c r="C47" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="12" t="s">
+      <c r="D47" s="14"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H47" s="12" t="s">
+      <c r="H47" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I47" s="13" t="s">
+      <c r="I47" s="14" t="s">
         <v>192</v>
       </c>
       <c r="J47" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="K47" s="12"/>
+      <c r="K47" s="13"/>
       <c r="L47" s="6"/>
-      <c r="M47" s="13"/>
+      <c r="M47" s="14"/>
       <c r="N47" s="11" t="s">
         <v>50</v>
       </c>
@@ -4262,24 +4306,24 @@
       <c r="C48" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="D48" s="13"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="12" t="s">
+      <c r="D48" s="14"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H48" s="12" t="s">
+      <c r="H48" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I48" s="13" t="s">
+      <c r="I48" s="14" t="s">
         <v>197</v>
       </c>
       <c r="J48" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K48" s="12"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
       <c r="N48" s="11" t="s">
         <v>50</v>
       </c>
@@ -4297,24 +4341,24 @@
       <c r="C49" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="12" t="s">
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="12" t="s">
+      <c r="H49" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I49" s="13" t="s">
+      <c r="I49" s="14" t="s">
         <v>202</v>
       </c>
       <c r="J49" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="K49" s="12"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
       <c r="N49" s="11" t="s">
         <v>50</v>
       </c>
@@ -4332,24 +4376,24 @@
       <c r="C50" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="12" t="s">
+      <c r="D50" s="14"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H50" s="12" t="s">
+      <c r="H50" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I50" s="13" t="s">
+      <c r="I50" s="14" t="s">
         <v>207</v>
       </c>
       <c r="J50" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="K50" s="12"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="14"/>
       <c r="N50" s="11" t="s">
         <v>50</v>
       </c>
@@ -4358,22 +4402,22 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="13" t="s">
         <v>209</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="13" t="s">
         <v>93</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
       <c r="F51" s="19"/>
-      <c r="G51" s="12" t="s">
+      <c r="G51" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H51" s="12" t="s">
+      <c r="H51" s="13" t="s">
         <v>142</v>
       </c>
       <c r="I51" s="19"/>
@@ -4395,11 +4439,6 @@
       <c r="F52" s="19"/>
       <c r="G52" s="24"/>
       <c r="H52" s="23"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="25"/>
       <c r="N52" s="25"/>
       <c r="O52" s="23"/>
       <c r="P52" s="16"/>
@@ -4412,13 +4451,8 @@
       <c r="D53" s="23"/>
       <c r="E53" s="19"/>
       <c r="F53" s="19"/>
-      <c r="G53" s="12"/>
+      <c r="G53" s="13"/>
       <c r="H53" s="23"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
       <c r="N53" s="25"/>
       <c r="O53" s="23"/>
       <c r="P53" s="16"/>
@@ -4431,13 +4465,8 @@
       <c r="D54" s="23"/>
       <c r="E54" s="19"/>
       <c r="F54" s="19"/>
-      <c r="G54" s="12"/>
+      <c r="G54" s="13"/>
       <c r="H54" s="23"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
       <c r="N54" s="25"/>
       <c r="O54" s="23"/>
       <c r="P54" s="16"/>
@@ -4450,7 +4479,7 @@
       <c r="D55" s="23"/>
       <c r="E55" s="19"/>
       <c r="F55" s="19"/>
-      <c r="G55" s="12"/>
+      <c r="G55" s="13"/>
       <c r="H55" s="23"/>
       <c r="I55" s="25"/>
       <c r="J55" s="25"/>
@@ -4469,7 +4498,7 @@
       <c r="D56" s="23"/>
       <c r="E56" s="19"/>
       <c r="F56" s="19"/>
-      <c r="G56" s="12"/>
+      <c r="G56" s="13"/>
       <c r="H56" s="23"/>
       <c r="I56" s="25"/>
       <c r="J56" s="25"/>
@@ -4488,7 +4517,7 @@
       <c r="D57" s="23"/>
       <c r="E57" s="19"/>
       <c r="F57" s="19"/>
-      <c r="G57" s="12"/>
+      <c r="G57" s="13"/>
       <c r="H57" s="23"/>
       <c r="I57" s="25"/>
       <c r="J57" s="25"/>
@@ -4507,7 +4536,7 @@
       <c r="D58" s="23"/>
       <c r="E58" s="19"/>
       <c r="F58" s="19"/>
-      <c r="G58" s="12"/>
+      <c r="G58" s="13"/>
       <c r="H58" s="23"/>
       <c r="I58" s="25"/>
       <c r="J58" s="25"/>
@@ -4526,7 +4555,7 @@
       <c r="D59" s="23"/>
       <c r="E59" s="19"/>
       <c r="F59" s="19"/>
-      <c r="G59" s="12"/>
+      <c r="G59" s="13"/>
       <c r="H59" s="23"/>
       <c r="I59" s="25"/>
       <c r="J59" s="25"/>
@@ -4545,7 +4574,7 @@
       <c r="D60" s="23"/>
       <c r="E60" s="19"/>
       <c r="F60" s="19"/>
-      <c r="G60" s="12"/>
+      <c r="G60" s="13"/>
       <c r="H60" s="23"/>
       <c r="I60" s="25"/>
       <c r="J60" s="25"/>
@@ -4564,7 +4593,7 @@
       <c r="D61" s="23"/>
       <c r="E61" s="19"/>
       <c r="F61" s="19"/>
-      <c r="G61" s="12"/>
+      <c r="G61" s="13"/>
       <c r="H61" s="23"/>
       <c r="I61" s="25"/>
       <c r="J61" s="25"/>
@@ -4583,7 +4612,7 @@
       <c r="D62" s="23"/>
       <c r="E62" s="19"/>
       <c r="F62" s="19"/>
-      <c r="G62" s="12"/>
+      <c r="G62" s="13"/>
       <c r="H62" s="23"/>
       <c r="I62" s="25"/>
       <c r="J62" s="25"/>
@@ -4602,7 +4631,7 @@
       <c r="D63" s="23"/>
       <c r="E63" s="19"/>
       <c r="F63" s="19"/>
-      <c r="G63" s="12"/>
+      <c r="G63" s="13"/>
       <c r="H63" s="23"/>
       <c r="I63" s="25"/>
       <c r="J63" s="25"/>
@@ -4621,7 +4650,7 @@
       <c r="D64" s="23"/>
       <c r="E64" s="19"/>
       <c r="F64" s="19"/>
-      <c r="G64" s="12"/>
+      <c r="G64" s="13"/>
       <c r="H64" s="23"/>
       <c r="I64" s="25"/>
       <c r="J64" s="25"/>
@@ -4640,7 +4669,7 @@
       <c r="D65" s="23"/>
       <c r="E65" s="19"/>
       <c r="F65" s="19"/>
-      <c r="G65" s="12"/>
+      <c r="G65" s="13"/>
       <c r="H65" s="23"/>
       <c r="I65" s="25"/>
       <c r="J65" s="25"/>
@@ -4659,7 +4688,7 @@
       <c r="D66" s="23"/>
       <c r="E66" s="19"/>
       <c r="F66" s="19"/>
-      <c r="G66" s="12"/>
+      <c r="G66" s="13"/>
       <c r="H66" s="23"/>
       <c r="I66" s="25"/>
       <c r="J66" s="25"/>
@@ -4678,7 +4707,7 @@
       <c r="D67" s="23"/>
       <c r="E67" s="19"/>
       <c r="F67" s="19"/>
-      <c r="G67" s="12"/>
+      <c r="G67" s="13"/>
       <c r="H67" s="23"/>
       <c r="I67" s="25"/>
       <c r="J67" s="25"/>
@@ -4697,7 +4726,7 @@
       <c r="D68" s="23"/>
       <c r="E68" s="19"/>
       <c r="F68" s="19"/>
-      <c r="G68" s="12"/>
+      <c r="G68" s="13"/>
       <c r="H68" s="23"/>
       <c r="I68" s="25"/>
       <c r="J68" s="25"/>
@@ -4716,7 +4745,7 @@
       <c r="D69" s="23"/>
       <c r="E69" s="19"/>
       <c r="F69" s="19"/>
-      <c r="G69" s="12"/>
+      <c r="G69" s="13"/>
       <c r="H69" s="23"/>
       <c r="I69" s="25"/>
       <c r="J69" s="25"/>
@@ -4735,7 +4764,7 @@
       <c r="D70" s="23"/>
       <c r="E70" s="19"/>
       <c r="F70" s="19"/>
-      <c r="G70" s="12"/>
+      <c r="G70" s="13"/>
       <c r="H70" s="23"/>
       <c r="I70" s="25"/>
       <c r="J70" s="25"/>
@@ -4754,7 +4783,7 @@
       <c r="D71" s="26"/>
       <c r="E71" s="19"/>
       <c r="F71" s="19"/>
-      <c r="G71" s="12"/>
+      <c r="G71" s="13"/>
       <c r="H71" s="26"/>
       <c r="I71" s="26"/>
       <c r="J71" s="26"/>
@@ -4773,7 +4802,7 @@
       <c r="D72" s="26"/>
       <c r="E72" s="19"/>
       <c r="F72" s="19"/>
-      <c r="G72" s="12"/>
+      <c r="G72" s="13"/>
       <c r="H72" s="26"/>
       <c r="I72" s="26"/>
       <c r="J72" s="26"/>
@@ -4792,7 +4821,7 @@
       <c r="D73" s="26"/>
       <c r="E73" s="19"/>
       <c r="F73" s="19"/>
-      <c r="G73" s="12"/>
+      <c r="G73" s="13"/>
       <c r="H73" s="26"/>
       <c r="I73" s="26"/>
       <c r="J73" s="26"/>
@@ -4811,7 +4840,7 @@
       <c r="D74" s="26"/>
       <c r="E74" s="19"/>
       <c r="F74" s="19"/>
-      <c r="G74" s="12"/>
+      <c r="G74" s="13"/>
       <c r="H74" s="26"/>
       <c r="I74" s="26"/>
       <c r="J74" s="26"/>
@@ -4830,7 +4859,7 @@
       <c r="D75" s="26"/>
       <c r="E75" s="19"/>
       <c r="F75" s="19"/>
-      <c r="G75" s="12"/>
+      <c r="G75" s="13"/>
       <c r="H75" s="26"/>
       <c r="I75" s="26"/>
       <c r="J75" s="26"/>
@@ -4849,7 +4878,7 @@
       <c r="D76" s="26"/>
       <c r="E76" s="19"/>
       <c r="F76" s="19"/>
-      <c r="G76" s="12"/>
+      <c r="G76" s="13"/>
       <c r="H76" s="26"/>
       <c r="I76" s="26"/>
       <c r="J76" s="26"/>
@@ -4868,7 +4897,7 @@
       <c r="D77" s="26"/>
       <c r="E77" s="19"/>
       <c r="F77" s="19"/>
-      <c r="G77" s="12"/>
+      <c r="G77" s="13"/>
       <c r="H77" s="26"/>
       <c r="I77" s="26"/>
       <c r="J77" s="26"/>
@@ -4887,7 +4916,7 @@
       <c r="D78" s="26"/>
       <c r="E78" s="19"/>
       <c r="F78" s="19"/>
-      <c r="G78" s="12"/>
+      <c r="G78" s="13"/>
       <c r="H78" s="26"/>
       <c r="I78" s="26"/>
       <c r="J78" s="26"/>
@@ -4906,7 +4935,7 @@
       <c r="D79" s="26"/>
       <c r="E79" s="19"/>
       <c r="F79" s="19"/>
-      <c r="G79" s="12"/>
+      <c r="G79" s="13"/>
       <c r="H79" s="26"/>
       <c r="I79" s="26"/>
       <c r="J79" s="26"/>
@@ -4925,7 +4954,7 @@
       <c r="D80" s="26"/>
       <c r="E80" s="19"/>
       <c r="F80" s="19"/>
-      <c r="G80" s="12"/>
+      <c r="G80" s="13"/>
       <c r="H80" s="26"/>
       <c r="I80" s="26"/>
       <c r="J80" s="26"/>
@@ -4944,7 +4973,7 @@
       <c r="D81" s="26"/>
       <c r="E81" s="19"/>
       <c r="F81" s="19"/>
-      <c r="G81" s="12"/>
+      <c r="G81" s="13"/>
       <c r="H81" s="26"/>
       <c r="I81" s="26"/>
       <c r="J81" s="26"/>
@@ -4963,7 +4992,7 @@
       <c r="D82" s="26"/>
       <c r="E82" s="19"/>
       <c r="F82" s="19"/>
-      <c r="G82" s="12"/>
+      <c r="G82" s="13"/>
       <c r="H82" s="26"/>
       <c r="I82" s="26"/>
       <c r="J82" s="26"/>
@@ -4982,7 +5011,7 @@
       <c r="D83" s="26"/>
       <c r="E83" s="19"/>
       <c r="F83" s="19"/>
-      <c r="G83" s="12"/>
+      <c r="G83" s="13"/>
       <c r="H83" s="26"/>
       <c r="I83" s="26"/>
       <c r="J83" s="26"/>
@@ -5001,7 +5030,7 @@
       <c r="D84" s="26"/>
       <c r="E84" s="19"/>
       <c r="F84" s="19"/>
-      <c r="G84" s="12"/>
+      <c r="G84" s="13"/>
       <c r="H84" s="26"/>
       <c r="I84" s="26"/>
       <c r="J84" s="26"/>
@@ -5020,7 +5049,7 @@
       <c r="D85" s="26"/>
       <c r="E85" s="19"/>
       <c r="F85" s="19"/>
-      <c r="G85" s="12"/>
+      <c r="G85" s="13"/>
       <c r="H85" s="26"/>
       <c r="I85" s="26"/>
       <c r="J85" s="26"/>
@@ -5039,7 +5068,7 @@
       <c r="D86" s="26"/>
       <c r="E86" s="19"/>
       <c r="F86" s="19"/>
-      <c r="G86" s="12"/>
+      <c r="G86" s="13"/>
       <c r="H86" s="26"/>
       <c r="I86" s="26"/>
       <c r="J86" s="26"/>
@@ -5058,7 +5087,7 @@
       <c r="D87" s="26"/>
       <c r="E87" s="19"/>
       <c r="F87" s="19"/>
-      <c r="G87" s="12"/>
+      <c r="G87" s="13"/>
       <c r="H87" s="26"/>
       <c r="I87" s="26"/>
       <c r="J87" s="26"/>
@@ -5077,7 +5106,7 @@
       <c r="D88" s="26"/>
       <c r="E88" s="19"/>
       <c r="F88" s="19"/>
-      <c r="G88" s="12"/>
+      <c r="G88" s="13"/>
       <c r="H88" s="26"/>
       <c r="I88" s="26"/>
       <c r="J88" s="26"/>
@@ -5096,7 +5125,7 @@
       <c r="D89" s="26"/>
       <c r="E89" s="19"/>
       <c r="F89" s="19"/>
-      <c r="G89" s="12"/>
+      <c r="G89" s="13"/>
       <c r="H89" s="26"/>
       <c r="I89" s="26"/>
       <c r="J89" s="26"/>
@@ -5115,7 +5144,7 @@
       <c r="D90" s="26"/>
       <c r="E90" s="19"/>
       <c r="F90" s="19"/>
-      <c r="G90" s="12"/>
+      <c r="G90" s="13"/>
       <c r="H90" s="26"/>
       <c r="I90" s="26"/>
       <c r="J90" s="26"/>
@@ -5134,7 +5163,7 @@
       <c r="D91" s="26"/>
       <c r="E91" s="19"/>
       <c r="F91" s="19"/>
-      <c r="G91" s="12"/>
+      <c r="G91" s="13"/>
       <c r="H91" s="26"/>
       <c r="I91" s="26"/>
       <c r="J91" s="26"/>
@@ -5153,7 +5182,7 @@
       <c r="D92" s="26"/>
       <c r="E92" s="19"/>
       <c r="F92" s="19"/>
-      <c r="G92" s="12"/>
+      <c r="G92" s="13"/>
       <c r="H92" s="26"/>
       <c r="I92" s="26"/>
       <c r="J92" s="26"/>
@@ -5172,7 +5201,7 @@
       <c r="D93" s="26"/>
       <c r="E93" s="19"/>
       <c r="F93" s="19"/>
-      <c r="G93" s="12"/>
+      <c r="G93" s="13"/>
       <c r="H93" s="26"/>
       <c r="I93" s="26"/>
       <c r="J93" s="26"/>
@@ -5191,7 +5220,7 @@
       <c r="D94" s="26"/>
       <c r="E94" s="19"/>
       <c r="F94" s="19"/>
-      <c r="G94" s="12"/>
+      <c r="G94" s="13"/>
       <c r="H94" s="26"/>
       <c r="I94" s="26"/>
       <c r="J94" s="26"/>
@@ -5210,7 +5239,7 @@
       <c r="D95" s="26"/>
       <c r="E95" s="19"/>
       <c r="F95" s="19"/>
-      <c r="G95" s="12"/>
+      <c r="G95" s="13"/>
       <c r="H95" s="26"/>
       <c r="I95" s="26"/>
       <c r="J95" s="26"/>
@@ -5229,7 +5258,7 @@
       <c r="D96" s="26"/>
       <c r="E96" s="19"/>
       <c r="F96" s="19"/>
-      <c r="G96" s="12"/>
+      <c r="G96" s="13"/>
       <c r="H96" s="26"/>
       <c r="I96" s="26"/>
       <c r="J96" s="26"/>
@@ -5248,7 +5277,7 @@
       <c r="D97" s="26"/>
       <c r="E97" s="19"/>
       <c r="F97" s="19"/>
-      <c r="G97" s="12"/>
+      <c r="G97" s="13"/>
       <c r="H97" s="26"/>
       <c r="I97" s="26"/>
       <c r="J97" s="26"/>
@@ -5267,7 +5296,7 @@
       <c r="D98" s="26"/>
       <c r="E98" s="19"/>
       <c r="F98" s="19"/>
-      <c r="G98" s="12"/>
+      <c r="G98" s="13"/>
       <c r="H98" s="26"/>
       <c r="I98" s="26"/>
       <c r="J98" s="26"/>
@@ -5286,7 +5315,7 @@
       <c r="D99" s="26"/>
       <c r="E99" s="19"/>
       <c r="F99" s="19"/>
-      <c r="G99" s="12"/>
+      <c r="G99" s="13"/>
       <c r="H99" s="26"/>
       <c r="I99" s="26"/>
       <c r="J99" s="26"/>
@@ -5305,7 +5334,7 @@
       <c r="D100" s="26"/>
       <c r="E100" s="19"/>
       <c r="F100" s="19"/>
-      <c r="G100" s="12"/>
+      <c r="G100" s="13"/>
       <c r="H100" s="26"/>
       <c r="I100" s="26"/>
       <c r="J100" s="26"/>
@@ -5324,7 +5353,7 @@
       <c r="D101" s="26"/>
       <c r="E101" s="19"/>
       <c r="F101" s="19"/>
-      <c r="G101" s="12"/>
+      <c r="G101" s="13"/>
       <c r="H101" s="26"/>
       <c r="I101" s="26"/>
       <c r="J101" s="26"/>
@@ -5343,7 +5372,7 @@
       <c r="D102" s="26"/>
       <c r="E102" s="19"/>
       <c r="F102" s="19"/>
-      <c r="G102" s="12"/>
+      <c r="G102" s="13"/>
       <c r="H102" s="26"/>
       <c r="I102" s="26"/>
       <c r="J102" s="26"/>
@@ -5362,7 +5391,7 @@
       <c r="D103" s="26"/>
       <c r="E103" s="19"/>
       <c r="F103" s="19"/>
-      <c r="G103" s="12"/>
+      <c r="G103" s="13"/>
       <c r="H103" s="26"/>
       <c r="I103" s="26"/>
       <c r="J103" s="26"/>
@@ -5381,7 +5410,7 @@
       <c r="D104" s="26"/>
       <c r="E104" s="19"/>
       <c r="F104" s="19"/>
-      <c r="G104" s="12"/>
+      <c r="G104" s="13"/>
       <c r="H104" s="26"/>
       <c r="I104" s="26"/>
       <c r="J104" s="26"/>
@@ -5400,7 +5429,7 @@
       <c r="D105" s="26"/>
       <c r="E105" s="19"/>
       <c r="F105" s="19"/>
-      <c r="G105" s="12"/>
+      <c r="G105" s="13"/>
       <c r="H105" s="26"/>
       <c r="I105" s="26"/>
       <c r="J105" s="26"/>
@@ -5419,7 +5448,7 @@
       <c r="D106" s="26"/>
       <c r="E106" s="19"/>
       <c r="F106" s="19"/>
-      <c r="G106" s="12"/>
+      <c r="G106" s="13"/>
       <c r="H106" s="26"/>
       <c r="I106" s="26"/>
       <c r="J106" s="26"/>
@@ -5438,7 +5467,7 @@
       <c r="D107" s="26"/>
       <c r="E107" s="19"/>
       <c r="F107" s="19"/>
-      <c r="G107" s="12"/>
+      <c r="G107" s="13"/>
       <c r="H107" s="26"/>
       <c r="I107" s="26"/>
       <c r="J107" s="26"/>
@@ -5457,7 +5486,7 @@
       <c r="D108" s="26"/>
       <c r="E108" s="19"/>
       <c r="F108" s="19"/>
-      <c r="G108" s="12"/>
+      <c r="G108" s="13"/>
       <c r="H108" s="26"/>
       <c r="I108" s="26"/>
       <c r="J108" s="26"/>
@@ -5476,7 +5505,7 @@
       <c r="D109" s="26"/>
       <c r="E109" s="19"/>
       <c r="F109" s="19"/>
-      <c r="G109" s="12"/>
+      <c r="G109" s="13"/>
       <c r="H109" s="26"/>
       <c r="I109" s="26"/>
       <c r="J109" s="26"/>
@@ -5495,7 +5524,7 @@
       <c r="D110" s="26"/>
       <c r="E110" s="19"/>
       <c r="F110" s="19"/>
-      <c r="G110" s="12"/>
+      <c r="G110" s="13"/>
       <c r="H110" s="26"/>
       <c r="I110" s="26"/>
       <c r="J110" s="26"/>
@@ -5514,7 +5543,7 @@
       <c r="D111" s="26"/>
       <c r="E111" s="19"/>
       <c r="F111" s="19"/>
-      <c r="G111" s="12"/>
+      <c r="G111" s="13"/>
       <c r="H111" s="26"/>
       <c r="I111" s="26"/>
       <c r="J111" s="26"/>
@@ -5533,7 +5562,7 @@
       <c r="D112" s="26"/>
       <c r="E112" s="19"/>
       <c r="F112" s="19"/>
-      <c r="G112" s="12"/>
+      <c r="G112" s="13"/>
       <c r="H112" s="26"/>
       <c r="I112" s="26"/>
       <c r="J112" s="26"/>
@@ -5552,7 +5581,7 @@
       <c r="D113" s="26"/>
       <c r="E113" s="19"/>
       <c r="F113" s="19"/>
-      <c r="G113" s="12"/>
+      <c r="G113" s="13"/>
       <c r="H113" s="26"/>
       <c r="I113" s="26"/>
       <c r="J113" s="26"/>
@@ -5571,7 +5600,7 @@
       <c r="D114" s="26"/>
       <c r="E114" s="19"/>
       <c r="F114" s="19"/>
-      <c r="G114" s="12"/>
+      <c r="G114" s="13"/>
       <c r="H114" s="26"/>
       <c r="I114" s="26"/>
       <c r="J114" s="26"/>
@@ -5590,7 +5619,7 @@
       <c r="D115" s="26"/>
       <c r="E115" s="19"/>
       <c r="F115" s="19"/>
-      <c r="G115" s="12"/>
+      <c r="G115" s="13"/>
       <c r="H115" s="26"/>
       <c r="I115" s="26"/>
       <c r="J115" s="26"/>
@@ -5609,7 +5638,7 @@
       <c r="D116" s="26"/>
       <c r="E116" s="19"/>
       <c r="F116" s="19"/>
-      <c r="G116" s="12"/>
+      <c r="G116" s="13"/>
       <c r="H116" s="26"/>
       <c r="I116" s="26"/>
       <c r="J116" s="26"/>
@@ -5628,7 +5657,7 @@
       <c r="D117" s="26"/>
       <c r="E117" s="19"/>
       <c r="F117" s="19"/>
-      <c r="G117" s="12"/>
+      <c r="G117" s="13"/>
       <c r="H117" s="26"/>
       <c r="I117" s="26"/>
       <c r="J117" s="26"/>
@@ -5647,7 +5676,7 @@
       <c r="D118" s="26"/>
       <c r="E118" s="19"/>
       <c r="F118" s="19"/>
-      <c r="G118" s="12"/>
+      <c r="G118" s="13"/>
       <c r="H118" s="26"/>
       <c r="I118" s="26"/>
       <c r="J118" s="26"/>
@@ -5666,7 +5695,7 @@
       <c r="D119" s="26"/>
       <c r="E119" s="19"/>
       <c r="F119" s="19"/>
-      <c r="G119" s="12"/>
+      <c r="G119" s="13"/>
       <c r="H119" s="26"/>
       <c r="I119" s="26"/>
       <c r="J119" s="26"/>
@@ -5685,7 +5714,7 @@
       <c r="D120" s="26"/>
       <c r="E120" s="19"/>
       <c r="F120" s="19"/>
-      <c r="G120" s="12"/>
+      <c r="G120" s="13"/>
       <c r="H120" s="26"/>
       <c r="I120" s="26"/>
       <c r="J120" s="26"/>
@@ -5704,7 +5733,7 @@
       <c r="D121" s="26"/>
       <c r="E121" s="19"/>
       <c r="F121" s="19"/>
-      <c r="G121" s="12"/>
+      <c r="G121" s="13"/>
       <c r="H121" s="26"/>
       <c r="I121" s="26"/>
       <c r="J121" s="26"/>
@@ -5723,7 +5752,7 @@
       <c r="D122" s="26"/>
       <c r="E122" s="19"/>
       <c r="F122" s="19"/>
-      <c r="G122" s="12"/>
+      <c r="G122" s="13"/>
       <c r="H122" s="26"/>
       <c r="I122" s="26"/>
       <c r="J122" s="26"/>
@@ -5742,7 +5771,7 @@
       <c r="D123" s="26"/>
       <c r="E123" s="19"/>
       <c r="F123" s="19"/>
-      <c r="G123" s="12"/>
+      <c r="G123" s="13"/>
       <c r="H123" s="26"/>
       <c r="I123" s="26"/>
       <c r="J123" s="26"/>
@@ -5761,7 +5790,7 @@
       <c r="D124" s="26"/>
       <c r="E124" s="19"/>
       <c r="F124" s="19"/>
-      <c r="G124" s="12"/>
+      <c r="G124" s="13"/>
       <c r="H124" s="26"/>
       <c r="I124" s="26"/>
       <c r="J124" s="26"/>
@@ -5780,7 +5809,7 @@
       <c r="D125" s="26"/>
       <c r="E125" s="19"/>
       <c r="F125" s="19"/>
-      <c r="G125" s="12"/>
+      <c r="G125" s="13"/>
       <c r="H125" s="26"/>
       <c r="I125" s="26"/>
       <c r="J125" s="26"/>
@@ -5799,7 +5828,7 @@
       <c r="D126" s="26"/>
       <c r="E126" s="19"/>
       <c r="F126" s="19"/>
-      <c r="G126" s="12"/>
+      <c r="G126" s="13"/>
       <c r="H126" s="26"/>
       <c r="I126" s="26"/>
       <c r="J126" s="26"/>
@@ -5818,7 +5847,7 @@
       <c r="D127" s="26"/>
       <c r="E127" s="19"/>
       <c r="F127" s="19"/>
-      <c r="G127" s="12"/>
+      <c r="G127" s="13"/>
       <c r="H127" s="26"/>
       <c r="I127" s="26"/>
       <c r="J127" s="26"/>
@@ -5837,7 +5866,7 @@
       <c r="D128" s="26"/>
       <c r="E128" s="19"/>
       <c r="F128" s="19"/>
-      <c r="G128" s="12"/>
+      <c r="G128" s="13"/>
       <c r="H128" s="26"/>
       <c r="I128" s="26"/>
       <c r="J128" s="26"/>
@@ -5856,7 +5885,7 @@
       <c r="D129" s="26"/>
       <c r="E129" s="19"/>
       <c r="F129" s="19"/>
-      <c r="G129" s="12"/>
+      <c r="G129" s="13"/>
       <c r="H129" s="26"/>
       <c r="I129" s="26"/>
       <c r="J129" s="26"/>
@@ -5875,7 +5904,7 @@
       <c r="D130" s="26"/>
       <c r="E130" s="19"/>
       <c r="F130" s="19"/>
-      <c r="G130" s="12"/>
+      <c r="G130" s="13"/>
       <c r="H130" s="26"/>
       <c r="I130" s="26"/>
       <c r="J130" s="26"/>
@@ -5894,7 +5923,7 @@
       <c r="D131" s="26"/>
       <c r="E131" s="19"/>
       <c r="F131" s="19"/>
-      <c r="G131" s="12"/>
+      <c r="G131" s="13"/>
       <c r="H131" s="26"/>
       <c r="I131" s="26"/>
       <c r="J131" s="26"/>
@@ -5913,7 +5942,7 @@
       <c r="D132" s="26"/>
       <c r="E132" s="19"/>
       <c r="F132" s="19"/>
-      <c r="G132" s="12"/>
+      <c r="G132" s="13"/>
       <c r="H132" s="26"/>
       <c r="I132" s="26"/>
       <c r="J132" s="26"/>
@@ -5932,7 +5961,7 @@
       <c r="D133" s="26"/>
       <c r="E133" s="19"/>
       <c r="F133" s="19"/>
-      <c r="G133" s="12"/>
+      <c r="G133" s="13"/>
       <c r="H133" s="26"/>
       <c r="I133" s="26"/>
       <c r="J133" s="26"/>
@@ -5946,21 +5975,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="P2:P7"/>
-    <mergeCell ref="Q2:Q7"/>
-    <mergeCell ref="Q8:Q13"/>
+    <mergeCell ref="Q21:Q27"/>
+    <mergeCell ref="R21:R27"/>
+    <mergeCell ref="P28:P34"/>
     <mergeCell ref="Q28:Q34"/>
     <mergeCell ref="R28:R34"/>
     <mergeCell ref="P35:P51"/>
     <mergeCell ref="Q35:Q51"/>
     <mergeCell ref="R35:R51"/>
+    <mergeCell ref="P2:P7"/>
+    <mergeCell ref="Q2:Q7"/>
     <mergeCell ref="P8:P13"/>
+    <mergeCell ref="Q8:Q13"/>
     <mergeCell ref="P14:P20"/>
     <mergeCell ref="Q14:Q20"/>
     <mergeCell ref="P21:P27"/>
-    <mergeCell ref="Q21:Q27"/>
-    <mergeCell ref="R21:R27"/>
-    <mergeCell ref="P28:P34"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6033,25 +6062,25 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>213</v>
       </c>
       <c r="D2" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H2" s="25" t="s">
@@ -6070,29 +6099,29 @@
       <c r="O2" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="P2" s="12"/>
+      <c r="P2" s="13"/>
       <c r="Q2" s="10"/>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="25" t="s">
@@ -6113,25 +6142,25 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="25" t="s">
@@ -6152,266 +6181,266 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="14" t="s">
         <v>231</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="K5" s="13"/>
+      <c r="K5" s="14"/>
       <c r="L5" s="11">
         <v>27.0</v>
       </c>
       <c r="M5" s="11">
         <v>1020.0</v>
       </c>
-      <c r="N5" s="13"/>
+      <c r="N5" s="14"/>
       <c r="O5" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="14" t="s">
         <v>239</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
       <c r="O6" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="14" t="s">
         <v>239</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
       <c r="O7" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="14" t="s">
         <v>253</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
       <c r="O8" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="14" t="s">
         <v>261</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
       <c r="O9" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="14" t="s">
         <v>269</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
       <c r="O10" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="13" t="s">
         <v>273</v>
       </c>
       <c r="I11" s="27" t="s">
@@ -6431,274 +6460,274 @@
       <c r="Q11" s="10"/>
     </row>
     <row r="12">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="14" t="s">
         <v>220</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
       <c r="O12" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="14" t="s">
         <v>224</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
       <c r="O13" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="14" t="s">
         <v>231</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
       <c r="O14" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="14" t="s">
         <v>239</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
       <c r="O15" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="14" t="s">
         <v>253</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
       <c r="O16" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="14" t="s">
         <v>261</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
       <c r="O17" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="14" t="s">
         <v>269</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
       <c r="O18" s="28" t="s">
         <v>216</v>
       </c>
@@ -6809,7 +6838,7 @@
       <c r="D3" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F3" s="23">
@@ -6837,7 +6866,7 @@
       <c r="D4" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F4" s="23">
@@ -6865,7 +6894,7 @@
       <c r="D5" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F5" s="23">
@@ -6893,7 +6922,7 @@
       <c r="D6" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F6" s="23">
@@ -6921,7 +6950,7 @@
       <c r="D7" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F7" s="23">
@@ -6949,7 +6978,7 @@
       <c r="D8" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F8" s="23">
@@ -6977,7 +7006,7 @@
       <c r="D9" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F9" s="23">
@@ -7005,7 +7034,7 @@
       <c r="D10" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F10" s="23">
@@ -7033,7 +7062,7 @@
       <c r="D11" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F11" s="23">
@@ -7061,7 +7090,7 @@
       <c r="D12" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F12" s="23">
@@ -7089,7 +7118,7 @@
       <c r="D13" s="23" t="s">
         <v>320</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F13" s="23">
@@ -7117,7 +7146,7 @@
       <c r="D14" s="23" t="s">
         <v>322</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F14" s="23">
@@ -7145,7 +7174,7 @@
       <c r="D15" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F15" s="23">
@@ -7173,7 +7202,7 @@
       <c r="D16" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F16" s="23">
@@ -7201,7 +7230,7 @@
       <c r="D17" s="23" t="s">
         <v>328</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F17" s="23">
@@ -7229,7 +7258,7 @@
       <c r="D18" s="23" t="s">
         <v>330</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F18" s="23">
@@ -7257,7 +7286,7 @@
       <c r="D19" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F19" s="23">
@@ -7285,7 +7314,7 @@
       <c r="D20" s="23" t="s">
         <v>334</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F20" s="23">
@@ -7313,7 +7342,7 @@
       <c r="D21" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F21" s="26">
@@ -7341,7 +7370,7 @@
       <c r="D22" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F22" s="26">
@@ -7369,7 +7398,7 @@
       <c r="D23" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F23" s="26">
@@ -7397,7 +7426,7 @@
       <c r="D24" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F24" s="26">
@@ -7425,7 +7454,7 @@
       <c r="D25" s="26" t="s">
         <v>345</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F25" s="26">
@@ -7453,7 +7482,7 @@
       <c r="D26" s="26" t="s">
         <v>347</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F26" s="26">
@@ -7481,7 +7510,7 @@
       <c r="D27" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F27" s="26">
@@ -7509,7 +7538,7 @@
       <c r="D28" s="26" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F28" s="26">
@@ -7537,7 +7566,7 @@
       <c r="D29" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F29" s="26">
@@ -7565,7 +7594,7 @@
       <c r="D30" s="26" t="s">
         <v>355</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F30" s="26">
@@ -7593,7 +7622,7 @@
       <c r="D31" s="26" t="s">
         <v>357</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F31" s="26">
@@ -7621,7 +7650,7 @@
       <c r="D32" s="26" t="s">
         <v>359</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F32" s="26">
@@ -7649,7 +7678,7 @@
       <c r="D33" s="26" t="s">
         <v>361</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F33" s="26">
@@ -7677,7 +7706,7 @@
       <c r="D34" s="26" t="s">
         <v>363</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F34" s="26">
@@ -7705,7 +7734,7 @@
       <c r="D35" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F35" s="26">
@@ -7733,7 +7762,7 @@
       <c r="D36" s="26" t="s">
         <v>367</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F36" s="26">
@@ -7761,7 +7790,7 @@
       <c r="D37" s="26" t="s">
         <v>369</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F37" s="26">
@@ -7789,7 +7818,7 @@
       <c r="D38" s="26" t="s">
         <v>371</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F38" s="26">
@@ -7817,7 +7846,7 @@
       <c r="D39" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F39" s="26">
@@ -7845,7 +7874,7 @@
       <c r="D40" s="26" t="s">
         <v>375</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F40" s="26">
@@ -7873,7 +7902,7 @@
       <c r="D41" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F41" s="26">
@@ -7901,7 +7930,7 @@
       <c r="D42" s="26" t="s">
         <v>378</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F42" s="26">
@@ -7929,7 +7958,7 @@
       <c r="D43" s="26" t="s">
         <v>380</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F43" s="26">
@@ -7957,7 +7986,7 @@
       <c r="D44" s="26" t="s">
         <v>382</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F44" s="26">
@@ -7985,7 +8014,7 @@
       <c r="D45" s="26" t="s">
         <v>384</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F45" s="26">
@@ -8013,7 +8042,7 @@
       <c r="D46" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F46" s="26">
@@ -8041,7 +8070,7 @@
       <c r="D47" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F47" s="26">
@@ -8069,7 +8098,7 @@
       <c r="D48" s="26" t="s">
         <v>390</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F48" s="26">
@@ -8097,7 +8126,7 @@
       <c r="D49" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F49" s="26">
@@ -8125,7 +8154,7 @@
       <c r="D50" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F50" s="26">
@@ -8153,7 +8182,7 @@
       <c r="D51" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F51" s="26">
@@ -8181,7 +8210,7 @@
       <c r="D52" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F52" s="26">
@@ -8209,7 +8238,7 @@
       <c r="D53" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F53" s="26">
@@ -8237,7 +8266,7 @@
       <c r="D54" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F54" s="26">
@@ -8265,7 +8294,7 @@
       <c r="D55" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F55" s="26">
@@ -8293,7 +8322,7 @@
       <c r="D56" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F56" s="26">
@@ -8321,7 +8350,7 @@
       <c r="D57" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E57" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F57" s="26">
@@ -8349,7 +8378,7 @@
       <c r="D58" s="26" t="s">
         <v>402</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F58" s="26">
@@ -8377,7 +8406,7 @@
       <c r="D59" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="E59" s="12" t="s">
+      <c r="E59" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F59" s="26">
@@ -8402,7 +8431,7 @@
       <c r="C60" s="26">
         <v>59.0</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E60" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F60" s="26">
@@ -8430,7 +8459,7 @@
       <c r="D61" s="26" t="s">
         <v>406</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F61" s="26">
@@ -8458,7 +8487,7 @@
       <c r="D62" s="26" t="s">
         <v>408</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E62" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F62" s="26">
@@ -8483,7 +8512,7 @@
       <c r="C63" s="26">
         <v>62.0</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E63" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F63" s="26">
@@ -8511,7 +8540,7 @@
       <c r="D64" s="26" t="s">
         <v>411</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F64" s="26">
@@ -8539,7 +8568,7 @@
       <c r="D65" s="26" t="s">
         <v>413</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E65" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F65" s="26">
@@ -8567,7 +8596,7 @@
       <c r="D66" s="26" t="s">
         <v>415</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F66" s="26">
@@ -8595,7 +8624,7 @@
       <c r="D67" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="E67" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F67" s="26">
@@ -8623,7 +8652,7 @@
       <c r="D68" s="26" t="s">
         <v>419</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F68" s="26">
@@ -8651,7 +8680,7 @@
       <c r="D69" s="26" t="s">
         <v>421</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F69" s="26">
@@ -8679,7 +8708,7 @@
       <c r="D70" s="26" t="s">
         <v>423</v>
       </c>
-      <c r="E70" s="12" t="s">
+      <c r="E70" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F70" s="26">
@@ -8707,7 +8736,7 @@
       <c r="D71" s="26" t="s">
         <v>425</v>
       </c>
-      <c r="E71" s="12" t="s">
+      <c r="E71" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F71" s="26">
@@ -8735,7 +8764,7 @@
       <c r="D72" s="26" t="s">
         <v>427</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E72" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F72" s="26">
@@ -8763,7 +8792,7 @@
       <c r="D73" s="26" t="s">
         <v>429</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F73" s="26">
@@ -8791,7 +8820,7 @@
       <c r="D74" s="26" t="s">
         <v>431</v>
       </c>
-      <c r="E74" s="12" t="s">
+      <c r="E74" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F74" s="26">
@@ -8819,7 +8848,7 @@
       <c r="D75" s="26" t="s">
         <v>433</v>
       </c>
-      <c r="E75" s="12" t="s">
+      <c r="E75" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F75" s="26">
@@ -8847,7 +8876,7 @@
       <c r="D76" s="26" t="s">
         <v>435</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E76" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F76" s="26">
@@ -8875,7 +8904,7 @@
       <c r="D77" s="26" t="s">
         <v>437</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F77" s="26">
@@ -8903,7 +8932,7 @@
       <c r="D78" s="26" t="s">
         <v>439</v>
       </c>
-      <c r="E78" s="12" t="s">
+      <c r="E78" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F78" s="26">
@@ -8931,7 +8960,7 @@
       <c r="D79" s="26" t="s">
         <v>441</v>
       </c>
-      <c r="E79" s="12" t="s">
+      <c r="E79" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F79" s="26">
@@ -8959,7 +8988,7 @@
       <c r="D80" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="E80" s="12" t="s">
+      <c r="E80" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F80" s="26">
@@ -8987,7 +9016,7 @@
       <c r="D81" s="26" t="s">
         <v>445</v>
       </c>
-      <c r="E81" s="12" t="s">
+      <c r="E81" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F81" s="26">
@@ -9015,7 +9044,7 @@
       <c r="D82" s="26" t="s">
         <v>447</v>
       </c>
-      <c r="E82" s="12" t="s">
+      <c r="E82" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F82" s="26">
@@ -9043,7 +9072,7 @@
       <c r="D83" s="26" t="s">
         <v>449</v>
       </c>
-      <c r="E83" s="12" t="s">
+      <c r="E83" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F83" s="26">
@@ -9071,7 +9100,7 @@
       <c r="D84" s="26" t="s">
         <v>451</v>
       </c>
-      <c r="E84" s="12" t="s">
+      <c r="E84" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F84" s="26">
@@ -9097,7 +9126,7 @@
       <c r="D85" s="26" t="s">
         <v>453</v>
       </c>
-      <c r="E85" s="12" t="s">
+      <c r="E85" s="13" t="s">
         <v>298</v>
       </c>
       <c r="F85" s="26">
@@ -9189,6 +9218,47 @@
         <v>24.350025</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>461</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25">
+        <v>25.0</v>
+      </c>
+      <c r="E14" s="12">
+        <v>7.0E7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="25"/>
+      <c r="B15" s="25" t="s">
+        <v>462</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25">
+        <v>27.0</v>
+      </c>
+      <c r="E15" s="12">
+        <v>2400000.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25" t="s">
+        <v>463</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25">
+        <v>25.0</v>
+      </c>
+      <c r="E16" s="12">
+        <v>6.7E7</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>